<commit_message>
emmat0 and emmatn understood
</commit_message>
<xml_diff>
--- a/experimental.xlsx
+++ b/experimental.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1763" uniqueCount="307">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1763" uniqueCount="308">
   <si>
     <t xml:space="preserve">Neha Original Recipe</t>
   </si>
@@ -369,511 +369,514 @@
     <t xml:space="preserve">2021/02/18</t>
   </si>
   <si>
+    <t xml:space="preserve">2021/02/22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">temp [C]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">time/rate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HP1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10min</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5min</t>
+  </si>
+  <si>
+    <t xml:space="preserve">60min</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HP2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NT1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0min</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2K/min</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1K/min</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NT2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NT3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3K/min</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NT4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4K/min</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NT5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NT6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NT7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sample</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Substrate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Seed layer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stiring time [h]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">layers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HEATING</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SEM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.0.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">glass</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test, heating rate max with scratch in middle, discarded </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2020/10/05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.1.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">frist sample, not entirely homogeneous</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.1.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">from room temperature (RT) orientation when blading ((0,0)(1,0), horizontal)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.1.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">from RT, ((0,0)(1,1), diagonal) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.1.4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">from RT, ((0,0)(0,1), vertical) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.1.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">from 40C ((0,0)(0,1), vertical)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2020/10/07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.2.6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ZnO2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">from 80C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.2.7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">steel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.2.8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.2.9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2020/10/08</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.2.10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">from 80C, didn’t stir and hole in parafilm for 10-20 hours </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.2.11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2020/10/09</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.2.12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.2.13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-1/1-3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">from 80C// second layer </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-2/1-3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.3.14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.3.15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FTO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">from 80C </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-1/1-3/1-4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">From 40 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-2/1-3/1-4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-3/1-4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.4.16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.4.17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2020/10/23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-2/1-4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">from 80C// second layer // TIXO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-4/1-4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.1.18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">from 80C // TIXO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.1.19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.1.20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.1.21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2020/10/27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">From 80-100-cool 2h-100-150…//TESA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.4.31</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.1.32</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.1.33</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.1.36</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.1.37</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2020/10/28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.4.30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">From 80C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2-1/2-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3-1/3-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2020/10/29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.4.22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.4.23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2020/10/30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2020/11/04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2020/11/05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2020/11/09</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2020/11/10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4-1/4-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">19.11.2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5-1/5-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6-1/6-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7-1/7-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2020/11/11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2020/11/12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2020/11/13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2020/11/16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2020/11/17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2020/11/18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2020/11/19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">double tape </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2020/11/20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2020/11/23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2020/11/24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">27.11.2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">runter gefallen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2020/11/30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">drop aged sol</t>
+  </si>
+  <si>
+    <t xml:space="preserve">03.12.2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5x</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2020/12/02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10x</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3x</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 days before calcination</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11x</t>
+  </si>
+  <si>
+    <t xml:space="preserve">doble conc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">spin coating</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18.01.2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">long sample</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5x/10x</t>
+  </si>
+  <si>
+    <t xml:space="preserve">long sample 24 tage pause</t>
+  </si>
+  <si>
+    <t xml:space="preserve">steel </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2x</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NT2 twice</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4F,HG,DOC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021/01/18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1x</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4F,HG,DOC,old(milky)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3F,HG,DOC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5F,HG,noDOC, noPYRO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5F,HG,noDOC </t>
+  </si>
+  <si>
+    <t xml:space="preserve">4F*,HG,DOC(milky)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4F,SC2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4x</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2F,vDOC=10</t>
+  </si>
+  <si>
     <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">temp [C]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">time/rate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HP1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10min</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5min</t>
-  </si>
-  <si>
-    <t xml:space="preserve">60min</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HP2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NT1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0min</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2K/min</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1K/min</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NT2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NT3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3K/min</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NT4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4K/min</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NT5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NT6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NT7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sample</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Substrate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Seed layer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stiring time [h]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">layers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HEATING</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SEM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.0.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">glass</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1-0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test, heating rate max with scratch in middle, discarded </t>
-  </si>
-  <si>
-    <t xml:space="preserve">2020/10/05</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.1.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1-1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">frist sample, not entirely homogeneous</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.1.2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">from room temperature (RT) orientation when blading ((0,0)(1,0), horizontal)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.1.3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">from RT, ((0,0)(1,1), diagonal) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.1.4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">from RT, ((0,0)(0,1), vertical) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.1.5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">from 40C ((0,0)(0,1), vertical)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2020/10/07</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.2.6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ZnO2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1-2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">from 80C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.2.7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">steel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.2.8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.2.9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2020/10/08</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.2.10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ITO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">from 80C, didn’t stir and hole in parafilm for 10-20 hours </t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.2.11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2020/10/09</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.2.12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.2.13</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1-1/1-3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">from 80C// second layer </t>
-  </si>
-  <si>
-    <t xml:space="preserve">1-2/1-3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.3.14</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1-3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.3.15</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FTO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">from 80C </t>
-  </si>
-  <si>
-    <t xml:space="preserve">1-1/1-3/1-4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">From 40 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">1-2/1-3/1-4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1-3/1-4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.4.16</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1-4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.4.17</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2020/10/23</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1-2/1-4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">from 80C// second layer // TIXO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1-4/1-4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.1.18</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2-1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">from 80C // TIXO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.1.19</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3.1.20</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3-1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3.1.21</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2020/10/27</t>
-  </si>
-  <si>
-    <t xml:space="preserve">From 80-100-cool 2h-100-150…//TESA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.4.31</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.1.32</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.1.33</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3.1.36</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3.1.37</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2020/10/28</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.4.30</t>
-  </si>
-  <si>
-    <t xml:space="preserve">From 80C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2-1/2-1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3-1/3-1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2020/10/29</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.4.22</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.4.23</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2020/10/30</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2020/11/04</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2020/11/05</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2020/11/09</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4-1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5-1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6-1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7-1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2020/11/10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4-1/4-1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">19.11.2020</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5-1/5-1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6-1/6-1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7-1/7-1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2020/11/11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2020/11/12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2020/11/13</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2020/11/16</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2020/11/17</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2020/11/18</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2020/11/19</t>
-  </si>
-  <si>
-    <t xml:space="preserve">double tape </t>
-  </si>
-  <si>
-    <t xml:space="preserve">2020/11/20</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2020/11/23</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2020/11/24</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8-1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9-1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10-1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11-1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12-1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">27.11.2020</t>
-  </si>
-  <si>
-    <t xml:space="preserve">13-1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">runter gefallen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">14-1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">15-1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">16-1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2020/11/30</t>
-  </si>
-  <si>
-    <t xml:space="preserve">drop aged sol</t>
-  </si>
-  <si>
-    <t xml:space="preserve">03.12.2020</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5x</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2020/12/02</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10x</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3x</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2 days before calcination</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11x</t>
-  </si>
-  <si>
-    <t xml:space="preserve">doble conc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">spin coating</t>
-  </si>
-  <si>
-    <t xml:space="preserve">18.01.2021</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">long sample</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5x/10x</t>
-  </si>
-  <si>
-    <t xml:space="preserve">long sample 24 tage pause</t>
-  </si>
-  <si>
-    <t xml:space="preserve">steel </t>
-  </si>
-  <si>
-    <t xml:space="preserve">2x</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NT2 twice</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4F,HG,DOC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2021/01/18</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1x</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4F,HG,DOC,old(milky)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3F,HG,DOC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0x</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5F,HG,noDOC, noPYRO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5F,HG,noDOC </t>
-  </si>
-  <si>
-    <t xml:space="preserve">4F*,HG,DOC(milky)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4F,SC2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4x</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2F,vDOC=10</t>
   </si>
   <si>
     <t xml:space="preserve">3F,VDOC=1</t>
@@ -2449,7 +2452,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B58" activeCellId="0" sqref="B58"/>
+      <selection pane="bottomLeft" activeCell="B59" activeCellId="0" sqref="B59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4564,16 +4567,34 @@
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="96" t="str">
+      <c r="A58" s="96" t="n">
         <f aca="false">IF(ISBLANK(H58),"", H58/(G58+L58)*(($G$13+$L$13)/$H$13))</f>
-        <v/>
-      </c>
-      <c r="B58" s="0" t="s">
+        <v>3.5</v>
+      </c>
+      <c r="B58" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="C58" s="103" t="n">
+        <f aca="false">IF(ISBLANK(H58),"",H58/G58*(G$13/H$13))</f>
+        <v>4.125</v>
+      </c>
+      <c r="D58" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="E58" s="0" t="s">
         <v>114</v>
       </c>
-      <c r="C58" s="103" t="str">
-        <f aca="false">IF(ISBLANK(H58),"",H58/G58*(G$13/H$13))</f>
-        <v/>
+      <c r="G58" s="0" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="H58" s="0" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="J58" s="0" t="n">
+        <v>0.025</v>
+      </c>
+      <c r="L58" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12078,7 +12099,7 @@
         <v>282</v>
       </c>
       <c r="L255" s="0" t="s">
-        <v>114</v>
+        <v>283</v>
       </c>
     </row>
     <row r="256" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12104,7 +12125,7 @@
         <v>127</v>
       </c>
       <c r="K256" s="0" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
     </row>
     <row r="257" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12127,7 +12148,7 @@
         <v>127</v>
       </c>
       <c r="K257" s="0" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
     </row>
     <row r="258" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12150,7 +12171,7 @@
         <v>127</v>
       </c>
       <c r="K258" s="0" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
     </row>
     <row r="259" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12176,7 +12197,7 @@
         <v>127</v>
       </c>
       <c r="K259" s="0" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
     </row>
     <row r="260" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12193,25 +12214,25 @@
         <v>127</v>
       </c>
       <c r="K260" s="0" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="M260" s="0" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="N260" s="0" t="s">
         <v>139</v>
       </c>
       <c r="O260" s="0" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="P260" s="0" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="Q260" s="0" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="R260" s="0" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
     </row>
     <row r="261" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12275,7 +12296,7 @@
         <v>281</v>
       </c>
       <c r="J262" s="0" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="M262" s="0" t="n">
         <v>1</v>
@@ -12316,7 +12337,7 @@
         <v>243</v>
       </c>
       <c r="J263" s="0" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="M263" s="0" t="n">
         <v>5</v>
@@ -12357,7 +12378,7 @@
         <v>281</v>
       </c>
       <c r="J264" s="0" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="M264" s="0" t="n">
         <v>5</v>
@@ -12380,7 +12401,7 @@
     </row>
     <row r="265" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A265" s="0" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="B265" s="0" t="n">
         <v>21</v>
@@ -12398,7 +12419,7 @@
         <v>255</v>
       </c>
       <c r="J265" s="0" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="M265" s="0" t="n">
         <v>1</v>
@@ -12421,7 +12442,7 @@
     </row>
     <row r="266" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A266" s="0" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="B266" s="0" t="n">
         <v>21</v>
@@ -12439,7 +12460,7 @@
         <v>257</v>
       </c>
       <c r="J266" s="0" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="M266" s="0" t="n">
         <v>1</v>
@@ -12462,7 +12483,7 @@
     </row>
     <row r="267" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A267" s="0" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="B267" s="0" t="n">
         <v>26</v>
@@ -12480,12 +12501,12 @@
         <v>255</v>
       </c>
       <c r="J267" s="0" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
     </row>
     <row r="268" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A268" s="0" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="B268" s="0" t="n">
         <v>26</v>
@@ -12503,7 +12524,7 @@
         <v>257</v>
       </c>
       <c r="J268" s="0" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
     </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -12536,24 +12557,24 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
     </row>
   </sheetData>
@@ -12588,21 +12609,21 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="C1" s="0" t="s">
+        <v>304</v>
+      </c>
+      <c r="D1" s="103" t="s">
         <v>303</v>
-      </c>
-      <c r="D1" s="103" t="s">
-        <v>302</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>10</v>
@@ -12614,7 +12635,7 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>5</v>
@@ -12626,7 +12647,7 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>1</v>
@@ -12672,7 +12693,7 @@
         <v>0.0100401606425703</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>114</v>
+        <v>283</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
2021-03-11 7374,5648,3956,2700 added to exp.xlsx
</commit_message>
<xml_diff>
--- a/experimental.xlsx
+++ b/experimental.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1822" uniqueCount="318">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1834" uniqueCount="319">
   <si>
     <t xml:space="preserve">Neha Original Recipe</t>
   </si>
@@ -943,6 +943,9 @@
   </si>
   <si>
     <t xml:space="preserve">9x</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021/03/11</t>
   </si>
   <si>
     <t xml:space="preserve">SC1</t>
@@ -5507,9 +5510,9 @@
   <dimension ref="A1:S1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A242" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A246" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A285" activeCellId="0" sqref="A285"/>
+      <selection pane="bottomLeft" activeCell="A289" activeCellId="0" sqref="A289"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -13407,6 +13410,170 @@
       </c>
       <c r="S284" s="0" t="n">
         <v>8318</v>
+      </c>
+    </row>
+    <row r="285" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A285" s="0" t="s">
+        <v>306</v>
+      </c>
+      <c r="B285" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="C285" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E285" s="0" t="n">
+        <v>217</v>
+      </c>
+      <c r="F285" s="0" t="s">
+        <v>171</v>
+      </c>
+      <c r="I285" s="0" t="s">
+        <v>264</v>
+      </c>
+      <c r="M285" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="N285" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="O285" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="P285" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="Q285" s="0" t="n">
+        <v>600</v>
+      </c>
+      <c r="R285" s="0" t="n">
+        <v>500</v>
+      </c>
+      <c r="S285" s="0" t="n">
+        <v>7374</v>
+      </c>
+    </row>
+    <row r="286" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A286" s="0" t="s">
+        <v>306</v>
+      </c>
+      <c r="B286" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="C286" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E286" s="0" t="n">
+        <v>214</v>
+      </c>
+      <c r="F286" s="0" t="s">
+        <v>171</v>
+      </c>
+      <c r="I286" s="0" t="s">
+        <v>303</v>
+      </c>
+      <c r="M286" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="N286" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="O286" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="P286" s="0" t="n">
+        <v>60</v>
+      </c>
+      <c r="Q286" s="0" t="n">
+        <v>1080</v>
+      </c>
+      <c r="R286" s="0" t="n">
+        <v>400</v>
+      </c>
+      <c r="S286" s="0" t="n">
+        <v>5648</v>
+      </c>
+    </row>
+    <row r="287" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A287" s="0" t="s">
+        <v>306</v>
+      </c>
+      <c r="B287" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="C287" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E287" s="0" t="n">
+        <v>215</v>
+      </c>
+      <c r="F287" s="0" t="s">
+        <v>171</v>
+      </c>
+      <c r="I287" s="0" t="s">
+        <v>264</v>
+      </c>
+      <c r="M287" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="N287" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="O287" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="P287" s="0" t="n">
+        <v>60</v>
+      </c>
+      <c r="Q287" s="0" t="n">
+        <v>360</v>
+      </c>
+      <c r="R287" s="0" t="n">
+        <v>300</v>
+      </c>
+      <c r="S287" s="0" t="n">
+        <v>3956</v>
+      </c>
+    </row>
+    <row r="288" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A288" s="0" t="s">
+        <v>306</v>
+      </c>
+      <c r="B288" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="C288" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E288" s="0" t="n">
+        <v>216</v>
+      </c>
+      <c r="F288" s="0" t="s">
+        <v>171</v>
+      </c>
+      <c r="I288" s="0" t="s">
+        <v>304</v>
+      </c>
+      <c r="M288" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="N288" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="O288" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="P288" s="0" t="n">
+        <v>60</v>
+      </c>
+      <c r="Q288" s="0" t="n">
+        <v>1080</v>
+      </c>
+      <c r="R288" s="0" t="n">
+        <v>300</v>
+      </c>
+      <c r="S288" s="0" t="n">
+        <v>2700</v>
       </c>
     </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -13439,24 +13606,24 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
     </row>
   </sheetData>
@@ -13491,21 +13658,21 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="C1" s="0" t="s">
+        <v>315</v>
+      </c>
+      <c r="D1" s="103" t="s">
         <v>314</v>
-      </c>
-      <c r="D1" s="103" t="s">
-        <v>313</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>10</v>
@@ -13517,7 +13684,7 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>5</v>
@@ -13529,7 +13696,7 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>1</v>

</xml_diff>

<commit_message>
pictures of DB++ and preliminary study pyDOE
</commit_message>
<xml_diff>
--- a/experimental.xlsx
+++ b/experimental.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" state="visible" r:id="rId2"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1914" uniqueCount="328">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1915" uniqueCount="329">
   <si>
     <t xml:space="preserve">Neha Original Recipe</t>
   </si>
@@ -952,6 +952,9 @@
   </si>
   <si>
     <t xml:space="preserve">Tcal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">make_exps.py ? </t>
   </si>
   <si>
     <t xml:space="preserve">/</t>
@@ -1904,7 +1907,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6796875" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.6953125" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="6.01"/>
@@ -2554,13 +2557,13 @@
   </sheetPr>
   <dimension ref="A1:O84"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="M19" activeCellId="0" sqref="M19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.6953125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="96" width="4.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="6.36"/>
@@ -5283,7 +5286,7 @@
       <selection pane="topLeft" activeCell="F10" activeCellId="0" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="101" width="9.47"/>
@@ -5735,15 +5738,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:S1048576"/>
+  <dimension ref="A1:T1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A176" activePane="bottomLeft" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A243" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="M260" activeCellId="0" sqref="M260"/>
+      <selection pane="bottomLeft" activeCell="T262" activeCellId="0" sqref="T262"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5234375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="2.77"/>
@@ -12740,6 +12743,9 @@
       <c r="R261" s="0" t="n">
         <v>400</v>
       </c>
+      <c r="T261" s="0" t="s">
+        <v>309</v>
+      </c>
     </row>
     <row r="262" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A262" s="0" t="s">
@@ -12761,7 +12767,7 @@
         <v>296</v>
       </c>
       <c r="J262" s="0" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="M262" s="0" t="n">
         <v>1</v>
@@ -12802,7 +12808,7 @@
         <v>258</v>
       </c>
       <c r="J263" s="0" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="M263" s="0" t="n">
         <v>5</v>
@@ -12843,7 +12849,7 @@
         <v>296</v>
       </c>
       <c r="J264" s="0" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="M264" s="0" t="n">
         <v>5</v>
@@ -12884,7 +12890,7 @@
         <v>270</v>
       </c>
       <c r="J265" s="0" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="M265" s="0" t="n">
         <v>1</v>
@@ -12925,7 +12931,7 @@
         <v>272</v>
       </c>
       <c r="J266" s="0" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="M266" s="0" t="n">
         <v>1</v>
@@ -12966,7 +12972,7 @@
         <v>270</v>
       </c>
       <c r="J267" s="0" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="M267" s="0" t="n">
         <v>5</v>
@@ -13007,7 +13013,7 @@
         <v>272</v>
       </c>
       <c r="J268" s="0" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="M268" s="0" t="n">
         <v>5</v>
@@ -13045,7 +13051,7 @@
         <v>179</v>
       </c>
       <c r="I269" s="0" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="M269" s="0" t="n">
         <v>2</v>
@@ -13083,7 +13089,7 @@
         <v>179</v>
       </c>
       <c r="I270" s="0" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="M270" s="0" t="n">
         <v>2</v>
@@ -13121,7 +13127,7 @@
         <v>179</v>
       </c>
       <c r="I271" s="0" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="M271" s="0" t="n">
         <v>4</v>
@@ -13185,7 +13191,7 @@
         <v>179</v>
       </c>
       <c r="I273" s="0" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="M273" s="0" t="n">
         <v>1</v>
@@ -13255,7 +13261,7 @@
         <v>179</v>
       </c>
       <c r="I275" s="0" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="M275" s="0" t="n">
         <v>4</v>
@@ -13293,7 +13299,7 @@
         <v>179</v>
       </c>
       <c r="I276" s="0" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="M276" s="0" t="n">
         <v>4</v>
@@ -13331,7 +13337,7 @@
         <v>179</v>
       </c>
       <c r="I277" s="0" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="M277" s="0" t="n">
         <v>4</v>
@@ -13410,7 +13416,7 @@
         <v>179</v>
       </c>
       <c r="I279" s="0" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="M279" s="0" t="n">
         <v>3</v>
@@ -13451,7 +13457,7 @@
         <v>179</v>
       </c>
       <c r="I280" s="0" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="M280" s="0" t="n">
         <v>3</v>
@@ -13574,7 +13580,7 @@
         <v>179</v>
       </c>
       <c r="I283" s="0" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="M283" s="0" t="n">
         <v>4</v>
@@ -13615,7 +13621,7 @@
         <v>179</v>
       </c>
       <c r="I284" s="0" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="M284" s="0" t="n">
         <v>3</v>
@@ -13697,7 +13703,7 @@
         <v>179</v>
       </c>
       <c r="I286" s="0" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="M286" s="0" t="n">
         <v>5</v>
@@ -13779,7 +13785,7 @@
         <v>179</v>
       </c>
       <c r="I288" s="0" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="M288" s="0" t="n">
         <v>5</v>
@@ -13823,7 +13829,7 @@
         <v>284</v>
       </c>
       <c r="K289" s="0" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="M289" s="0" t="n">
         <v>2</v>
@@ -13908,7 +13914,7 @@
         <v>296</v>
       </c>
       <c r="K291" s="0" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="M291" s="0" t="n">
         <v>2</v>
@@ -14066,7 +14072,7 @@
         <v>179</v>
       </c>
       <c r="I295" s="0" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="M295" s="0" t="n">
         <v>5</v>
@@ -14271,7 +14277,7 @@
         <v>179</v>
       </c>
       <c r="I300" s="0" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="M300" s="0" t="n">
         <v>5</v>
@@ -14353,7 +14359,7 @@
         <v>179</v>
       </c>
       <c r="I302" s="0" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="M302" s="0" t="n">
         <v>2</v>
@@ -14432,7 +14438,7 @@
         <v>179</v>
       </c>
       <c r="I304" s="0" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="M304" s="0" t="n">
         <v>5</v>
@@ -14473,7 +14479,7 @@
         <v>179</v>
       </c>
       <c r="I305" s="0" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="M305" s="0" t="n">
         <v>3</v>
@@ -14555,7 +14561,7 @@
         <v>179</v>
       </c>
       <c r="I307" s="0" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="M307" s="0" t="n">
         <v>4</v>
@@ -14596,7 +14602,7 @@
         <v>179</v>
       </c>
       <c r="I308" s="0" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="M308" s="0" t="n">
         <v>3</v>
@@ -14637,7 +14643,7 @@
         <v>179</v>
       </c>
       <c r="I309" s="0" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="M309" s="0" t="n">
         <v>2</v>
@@ -14766,28 +14772,28 @@
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
     </row>
   </sheetData>
@@ -14812,7 +14818,7 @@
       <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="5.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="103" width="8.06"/>
@@ -14820,21 +14826,21 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="C1" s="0" t="s">
+        <v>325</v>
+      </c>
+      <c r="D1" s="103" t="s">
         <v>324</v>
-      </c>
-      <c r="D1" s="103" t="s">
-        <v>323</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>10</v>
@@ -14846,7 +14852,7 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>5</v>
@@ -14858,7 +14864,7 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>1</v>

</xml_diff>